<commit_message>
added handling for plasmid, primers, water, master mix
</commit_message>
<xml_diff>
--- a/src/PCRProtocol/input.xlsx
+++ b/src/PCRProtocol/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohit/Documents/ropentrons/src/PCR Protocol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin2\Documents\Opentrons_iGEM\ropentrons\src\PCRProtocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFDDDBA-8BD9-1D42-81F2-7B8C9962197D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5252866-C36E-42B8-817E-4FD187B268A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="21540" windowHeight="14200" activeTab="2" xr2:uid="{CB1F6AAE-EA1C-254C-AED7-37271E944E0E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CB1F6AAE-EA1C-254C-AED7-37271E944E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="plasmids" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
   <si>
     <t>A</t>
   </si>
@@ -122,12 +122,6 @@
     <t>f_3</t>
   </si>
   <si>
-    <t>f_4</t>
-  </si>
-  <si>
-    <t>f_5</t>
-  </si>
-  <si>
     <t>p_1</t>
   </si>
   <si>
@@ -137,12 +131,6 @@
     <t>p_3</t>
   </si>
   <si>
-    <t>p_4</t>
-  </si>
-  <si>
-    <t>p_5</t>
-  </si>
-  <si>
     <t>r_1</t>
   </si>
   <si>
@@ -150,12 +138,6 @@
   </si>
   <si>
     <t>r_3</t>
-  </si>
-  <si>
-    <t>r_4</t>
-  </si>
-  <si>
-    <t>r_5</t>
   </si>
   <si>
     <t>notes</t>
@@ -184,12 +166,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -315,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -335,13 +323,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -362,8 +353,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -374,201 +371,447 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -769,23 +1012,23 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -840,6 +1083,226 @@
         <right style="thin">
           <color auto="1"/>
         </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top/>
         <bottom/>
         <vertical style="thin">
@@ -861,448 +1324,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
@@ -1663,6 +1684,36 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1685,36 +1736,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -1731,7 +1752,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2CD2D984-7FCC-2740-8445-11C83C723EC9}" name="Table3" displayName="Table3" ref="A1:M9" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="49" tableBorderDxfId="50" totalsRowBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2CD2D984-7FCC-2740-8445-11C83C723EC9}" name="Table3" displayName="Table3" ref="A1:M9" totalsRowShown="0" headerRowDxfId="50" headerRowBorderDxfId="49" tableBorderDxfId="48" totalsRowBorderDxfId="47">
   <autoFilter ref="A1:M9" xr:uid="{2CD2D984-7FCC-2740-8445-11C83C723EC9}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{DB1FCE51-FFEC-B340-AB1A-7C81EA2D1F44}" name="Plasmids" dataDxfId="46"/>
@@ -1753,37 +1774,37 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{974ADE0D-B41C-F846-A8CD-0924579E68FA}" name="Table35" displayName="Table35" ref="A1:M9" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{974ADE0D-B41C-F846-A8CD-0924579E68FA}" name="Table35" displayName="Table35" ref="A1:M9" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="A1:M9" xr:uid="{974ADE0D-B41C-F846-A8CD-0924579E68FA}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{73DA5924-F1D3-AE49-81DA-C4DEE0655D51}" name="Plasmids" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{870629C6-1ADD-2045-B8FA-69CF9A6619A9}" name="1" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{D36F33F6-77AB-1140-9E72-DEC051832333}" name="2" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{FFC3DA77-7526-D946-A2DD-7FDEBF04EE42}" name="3" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{56D78175-96D8-BB4D-B644-B3DB828482DE}" name="4" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{EC670162-3498-6B42-9F95-C3DD8ACAAF25}" name="5" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{DBA58EAE-91E9-D34D-91BD-15771BD05AF9}" name="6" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{BAFAB60B-AC62-B449-AA2D-7F5BDFB60838}" name="7" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{F954025D-80CF-314D-B9CA-391CAFFBE575}" name="8" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{D8A8DB3D-1B53-D741-A0BB-00FF7E91BADC}" name="9" dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{1227CF01-0933-B84E-AF7A-90800A9D1355}" name="10" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{1E6AE88D-89C0-EC4C-AD7C-D9995EE34253}" name="11" dataDxfId="19"/>
-    <tableColumn id="13" xr3:uid="{C461A632-51DD-FF4B-8696-19AF14C9CF49}" name="12" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{73DA5924-F1D3-AE49-81DA-C4DEE0655D51}" name="Plasmids" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{870629C6-1ADD-2045-B8FA-69CF9A6619A9}" name="1" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{D36F33F6-77AB-1140-9E72-DEC051832333}" name="2" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{FFC3DA77-7526-D946-A2DD-7FDEBF04EE42}" name="3" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{56D78175-96D8-BB4D-B644-B3DB828482DE}" name="4" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{EC670162-3498-6B42-9F95-C3DD8ACAAF25}" name="5" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{DBA58EAE-91E9-D34D-91BD-15771BD05AF9}" name="6" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{BAFAB60B-AC62-B449-AA2D-7F5BDFB60838}" name="7" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{F954025D-80CF-314D-B9CA-391CAFFBE575}" name="8" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{D8A8DB3D-1B53-D741-A0BB-00FF7E91BADC}" name="9" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{1227CF01-0933-B84E-AF7A-90800A9D1355}" name="10" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{1E6AE88D-89C0-EC4C-AD7C-D9995EE34253}" name="11" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{C461A632-51DD-FF4B-8696-19AF14C9CF49}" name="12" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AF33C09D-1F9D-FD4B-B479-D91954F5F374}" name="Table356" displayName="Table356" ref="A1:M9" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AF33C09D-1F9D-FD4B-B479-D91954F5F374}" name="Table356" displayName="Table356" ref="A1:M9" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="A1:M9" xr:uid="{AF33C09D-1F9D-FD4B-B479-D91954F5F374}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{4C267FA4-4529-FC43-BFD6-45CCECEAEE64}" name="Plasmids" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{6D37CEDB-C9DE-6744-BB7C-AE427B626E40}" name="1" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{005558E4-9BC7-8F4E-BC82-E4C6FF9DCCF1}" name="2" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{BDC6C965-42C3-2644-95BA-B74905AC59B7}" name="3" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{5E914549-B544-5A48-9F3A-6BB269733005}" name="4" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{BF2411D5-5898-164E-9968-74C539173E1E}" name="5" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{4C267FA4-4529-FC43-BFD6-45CCECEAEE64}" name="Plasmids" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{6D37CEDB-C9DE-6744-BB7C-AE427B626E40}" name="1" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{005558E4-9BC7-8F4E-BC82-E4C6FF9DCCF1}" name="2" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{BDC6C965-42C3-2644-95BA-B74905AC59B7}" name="3" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{5E914549-B544-5A48-9F3A-6BB269733005}" name="4" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{BF2411D5-5898-164E-9968-74C539173E1E}" name="5" dataDxfId="14"/>
     <tableColumn id="7" xr3:uid="{DE3A4D91-7A68-334C-B84A-2096BDBDF6B2}" name="6" dataDxfId="6"/>
     <tableColumn id="8" xr3:uid="{302F5F09-751F-7848-BA3C-E1A4EBE58497}" name="7" dataDxfId="5"/>
     <tableColumn id="9" xr3:uid="{F8127A6A-5CFF-2D42-9637-F4E6A95642C5}" name="8" dataDxfId="4"/>
@@ -2129,16 +2150,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF575A8-1323-2644-A31B-9AA9A92BE73C}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView zoomScale="50" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="20.83203125" customWidth="1"/>
+    <col min="1" max="13" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2179,30 +2200,30 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2212,14 +2233,14 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -2229,14 +2250,14 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2246,84 +2267,80 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2338,15 +2355,15 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView zoomScale="61" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="20.83203125" customWidth="1"/>
+    <col min="1" max="13" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2387,47 +2404,47 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -2437,14 +2454,14 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2454,84 +2471,80 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2545,16 +2558,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8ACE41-8C77-584F-B812-8E0443332E1E}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="63" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="20.83203125" customWidth="1"/>
+    <col min="1" max="13" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2595,30 +2608,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2628,31 +2635,37 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2662,84 +2675,80 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2751,21 +2760,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7460F568-3762-7245-8102-263373A4D556}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
@@ -2777,77 +2786,49 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>